<commit_message>
working on counting directors
</commit_message>
<xml_diff>
--- a/films.xlsx
+++ b/films.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,6 +41,12 @@
       <name val="Verdana"/>
       <b val="1"/>
       <color rgb="00FF6600"/>
+      <sz val="18"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <b val="1"/>
+      <color rgb="00FFFF99"/>
       <sz val="18"/>
     </font>
     <font>
@@ -83,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -91,7 +97,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -457,7 +464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +495,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B2" s="5" t="n"/>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Alien</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1979</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -496,7 +510,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n"/>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Predator</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1987</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
@@ -504,7 +525,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B4" s="5" t="n"/>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Inception</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2010</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
@@ -512,7 +540,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n"/>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Aliens</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1986</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -520,7 +555,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B6" s="5" t="n"/>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>The Lord of the Rings: The Two Towers</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2002</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
@@ -528,7 +570,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Collateral</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2004</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
@@ -536,7 +585,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B8" s="5" t="n"/>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>Batman Begins</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2005</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -544,7 +600,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B9" s="5" t="n"/>
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>The Dark Knight</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2008</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -552,7 +615,14 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>The Blues Brothers</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1980</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
@@ -1273,6 +1343,20 @@
         </is>
       </c>
       <c r="B100" s="5" t="n"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="6" t="inlineStr">
+        <is>
+          <t>Year with most Films</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="6" t="inlineStr">
+        <is>
+          <t>Most Films by Director</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
type error working on it
</commit_message>
<xml_diff>
--- a/films.xlsx
+++ b/films.xlsx
@@ -495,14 +495,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>Alien</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1979</v>
-      </c>
+      <c r="B2" s="5" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
@@ -510,14 +503,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>Predator</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1987</v>
-      </c>
+      <c r="B3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
@@ -525,14 +511,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>Inception</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2010</v>
-      </c>
+      <c r="B4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
@@ -540,14 +519,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>Aliens</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>1986</v>
-      </c>
+      <c r="B5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
@@ -555,14 +527,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>The Lord of the Rings: The Two Towers</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>2002</v>
-      </c>
+      <c r="B6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
@@ -570,14 +535,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>Collateral</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>2004</v>
-      </c>
+      <c r="B7" s="5" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
@@ -585,14 +543,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
-        <is>
-          <t>Batman Begins</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>2005</v>
-      </c>
+      <c r="B8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
@@ -600,14 +551,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
-        <is>
-          <t>The Dark Knight</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>2008</v>
-      </c>
+      <c r="B9" s="5" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
@@ -615,14 +559,7 @@
           <t>*</t>
         </is>
       </c>
-      <c r="B10" s="5" t="inlineStr">
-        <is>
-          <t>The Blues Brothers</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>1980</v>
-      </c>
+      <c r="B10" s="5" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">

</xml_diff>

<commit_message>
pivot table working, just need to get it working with other cells
</commit_message>
<xml_diff>
--- a/films.xlsx
+++ b/films.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tables" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Films" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Films" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -495,24 +494,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -567,11 +548,6 @@
       <c r="D2" t="n">
         <v>1979</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>$203,630,630</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Sci-Fi</t>
@@ -597,11 +573,6 @@
       <c r="D3" t="n">
         <v>1987</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>$38,532,010</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Sci-Fi</t>
@@ -626,11 +597,6 @@
       </c>
       <c r="D4" t="n">
         <v>2010</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>$825,532,764, 06 Jan 2011</t>
-        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>

</xml_diff>